<commit_message>
Looking good. Add 3 global_best variable
</commit_message>
<xml_diff>
--- a/結果比較表.xlsx
+++ b/結果比較表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\VRP_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA52080C-A104-45E5-8989-04332DDD9FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A4160B-2034-44C9-8D0A-4842449F0BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E8419044-2F44-49BB-AFDC-1F64E082A27B}"/>
   </bookViews>
@@ -265,31 +265,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -447,6 +427,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -457,61 +450,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -526,32 +513,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999919C6-E14E-4993-98A5-445A544D3785}">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -902,997 +895,997 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="K1" s="14" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="K1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="30" t="s">
+      <c r="M1" s="30"/>
+      <c r="N1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="2"/>
-      <c r="U1" s="14" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32"/>
+      <c r="U1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="W1" s="32"/>
-      <c r="X1" s="30" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="2"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="32"/>
     </row>
     <row r="2" spans="1:27" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="13" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="13" t="s">
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>8</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="15">
         <v>617.1</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <v>8</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="18">
         <v>618.29999999999995</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="3">
+      <c r="F3" s="19"/>
+      <c r="G3" s="1">
         <f>(E3-C3)/C3</f>
         <v>1.9445794846863259E-3</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="20">
-        <v>10</v>
-      </c>
-      <c r="M3" s="26">
+      <c r="L3" s="18">
+        <v>10</v>
+      </c>
+      <c r="M3" s="24">
         <v>828.94</v>
       </c>
-      <c r="N3" s="20">
-        <v>10</v>
-      </c>
-      <c r="O3" s="20">
+      <c r="N3" s="18">
+        <v>10</v>
+      </c>
+      <c r="O3" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="27">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="25">
         <f>(O3-M3)/M3</f>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="20">
+      <c r="V3" s="18">
         <v>14</v>
       </c>
-      <c r="W3" s="26">
+      <c r="W3" s="24">
         <v>1696.94</v>
       </c>
-      <c r="X3" s="20">
+      <c r="X3" s="18">
         <v>15</v>
       </c>
-      <c r="Y3" s="22">
+      <c r="Y3" s="20">
         <v>1663.15</v>
       </c>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="5">
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="3">
         <f>(Y3-W3)/W3</f>
         <v>-1.9912312751187409E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>7</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <v>547.1</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <v>7</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <v>548.1</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="3">
+      <c r="F4" s="19"/>
+      <c r="G4" s="1">
         <f t="shared" ref="G4:G14" si="0">(E4-C4)/C4</f>
         <v>1.8278194114421495E-3</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="20">
-        <v>10</v>
-      </c>
-      <c r="M4" s="17">
+      <c r="L4" s="18">
+        <v>10</v>
+      </c>
+      <c r="M4" s="15">
         <v>828.94</v>
       </c>
-      <c r="N4" s="20">
-        <v>10</v>
-      </c>
-      <c r="O4" s="20">
+      <c r="N4" s="18">
+        <v>10</v>
+      </c>
+      <c r="O4" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="27">
+      <c r="P4" s="18"/>
+      <c r="Q4" s="25">
         <f t="shared" ref="Q4:Q7" si="1">(O4-M4)/M4</f>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="U4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="20">
+      <c r="V4" s="18">
         <v>12</v>
       </c>
-      <c r="W4" s="17">
+      <c r="W4" s="15">
         <v>1554.75</v>
       </c>
-      <c r="X4" s="20">
+      <c r="X4" s="18">
         <v>14</v>
       </c>
-      <c r="Y4" s="22">
+      <c r="Y4" s="20">
         <v>1487.52</v>
       </c>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="5">
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="3">
         <f t="shared" ref="AA4:AA7" si="2">(Y4-W4)/W4</f>
         <v>-4.3241678726483372E-2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>5</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>454.6</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <v>4</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <v>473.4</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="3">
+      <c r="F5" s="19"/>
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>4.135503739551244E-2</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="20">
-        <v>10</v>
-      </c>
-      <c r="M5" s="17">
+      <c r="L5" s="18">
+        <v>10</v>
+      </c>
+      <c r="M5" s="15">
         <v>828.06</v>
       </c>
-      <c r="N5" s="20">
-        <v>10</v>
-      </c>
-      <c r="O5" s="20">
+      <c r="N5" s="18">
+        <v>10</v>
+      </c>
+      <c r="O5" s="18">
         <v>828.06500000000005</v>
       </c>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="27">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="25">
         <f t="shared" si="1"/>
         <v>6.0382097916927998E-6</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="20">
+      <c r="V5" s="18">
         <v>11</v>
       </c>
-      <c r="W5" s="17">
+      <c r="W5" s="15">
         <v>1261.67</v>
       </c>
-      <c r="X5" s="20">
+      <c r="X5" s="18">
         <v>12</v>
       </c>
-      <c r="Y5" s="20">
+      <c r="Y5" s="18">
         <v>1303.26</v>
       </c>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="5">
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="3">
         <f t="shared" si="2"/>
         <v>3.2964245801199929E-2</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>4</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="15">
         <v>416.9</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <v>4</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>418</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="3">
+      <c r="F6" s="19"/>
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>2.6385224274406878E-3</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="20">
-        <v>10</v>
-      </c>
-      <c r="M6" s="17">
+      <c r="L6" s="18">
+        <v>10</v>
+      </c>
+      <c r="M6" s="15">
         <v>824.78</v>
       </c>
-      <c r="N6" s="20">
-        <v>10</v>
-      </c>
-      <c r="O6" s="20">
+      <c r="N6" s="18">
+        <v>10</v>
+      </c>
+      <c r="O6" s="18">
         <v>824.77700000000004</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="27">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="25">
         <f t="shared" si="1"/>
         <v>-3.6373335919021552E-6</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="U6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="V6" s="20">
-        <v>10</v>
-      </c>
-      <c r="W6" s="17">
+      <c r="V6" s="18">
+        <v>10</v>
+      </c>
+      <c r="W6" s="15">
         <v>1135.48</v>
       </c>
-      <c r="X6" s="20">
-        <v>10</v>
-      </c>
-      <c r="Y6" s="20">
+      <c r="X6" s="18">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="18">
         <v>1140.8699999999999</v>
       </c>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="5">
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="3">
         <f t="shared" si="2"/>
         <v>4.7468911825834645E-3</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>530.5</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <v>5</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <v>556.70000000000005</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="3">
+      <c r="F7" s="19"/>
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>4.9387370405278123E-2</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="20">
-        <v>10</v>
-      </c>
-      <c r="M7" s="17">
+      <c r="L7" s="18">
+        <v>10</v>
+      </c>
+      <c r="M7" s="15">
         <v>828.94</v>
       </c>
-      <c r="N7" s="20">
-        <v>10</v>
-      </c>
-      <c r="O7" s="20">
+      <c r="N7" s="18">
+        <v>10</v>
+      </c>
+      <c r="O7" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="27">
+      <c r="P7" s="18"/>
+      <c r="Q7" s="25">
         <f t="shared" si="1"/>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="U7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="20">
+      <c r="V7" s="18">
         <v>13</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="15">
         <v>1629.44</v>
       </c>
-      <c r="X7" s="20">
+      <c r="X7" s="18">
         <v>15</v>
       </c>
-      <c r="Y7" s="22">
+      <c r="Y7" s="20">
         <v>1535.52</v>
       </c>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="5">
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="3">
         <f t="shared" si="2"/>
         <v>-5.7639434406912847E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="15">
         <v>465.4</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <v>5</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <v>466.5</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="3">
+      <c r="F8" s="19"/>
+      <c r="G8" s="1">
         <f>(E8-C8)/C8</f>
         <v>2.363558229480066E-3</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="20">
-        <v>10</v>
-      </c>
-      <c r="M8" s="17">
+      <c r="L8" s="18">
+        <v>10</v>
+      </c>
+      <c r="M8" s="15">
         <v>828.94</v>
       </c>
-      <c r="N8" s="20">
-        <v>10</v>
-      </c>
-      <c r="O8" s="20">
+      <c r="N8" s="18">
+        <v>10</v>
+      </c>
+      <c r="O8" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="27">
+      <c r="P8" s="18"/>
+      <c r="Q8" s="25">
         <f>(O8-M8)/M8</f>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U8" s="8" t="s">
+      <c r="U8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="18">
         <v>11</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="15">
         <v>1424.73</v>
       </c>
-      <c r="X8" s="20">
+      <c r="X8" s="18">
         <v>13</v>
       </c>
-      <c r="Y8" s="22">
+      <c r="Y8" s="20">
         <v>1382.58</v>
       </c>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="5">
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="3">
         <f>(Y8-W8)/W8</f>
         <v>-2.9584552862647724E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>4</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="15">
         <v>424.3</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="18">
         <v>4</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="18">
         <v>425.3</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="3">
+      <c r="F9" s="19"/>
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>2.3568230025925053E-3</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="20">
-        <v>10</v>
-      </c>
-      <c r="M9" s="17">
+      <c r="L9" s="18">
+        <v>10</v>
+      </c>
+      <c r="M9" s="15">
         <v>828.94</v>
       </c>
-      <c r="N9" s="20">
-        <v>10</v>
-      </c>
-      <c r="O9" s="20">
+      <c r="N9" s="18">
+        <v>10</v>
+      </c>
+      <c r="O9" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="27">
+      <c r="P9" s="18"/>
+      <c r="Q9" s="25">
         <f t="shared" ref="Q9:Q11" si="3">(O9-M9)/M9</f>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="U9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V9" s="20">
+      <c r="V9" s="18">
         <v>11</v>
       </c>
-      <c r="W9" s="17">
+      <c r="W9" s="15">
         <v>1230.48</v>
       </c>
-      <c r="X9" s="20">
+      <c r="X9" s="18">
         <v>11</v>
       </c>
-      <c r="Y9" s="20">
+      <c r="Y9" s="18">
         <v>1243.67</v>
       </c>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="5">
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="3">
         <f t="shared" ref="AA9:AA10" si="4">(Y9-W9)/W9</f>
         <v>1.0719394057603582E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="16">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14">
         <v>4</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="15">
         <v>397.3</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="18">
         <v>4</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="18">
         <v>398.3</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="3">
+      <c r="F10" s="19"/>
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>2.5169896803423106E-3</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="20">
-        <v>10</v>
-      </c>
-      <c r="M10" s="17">
+      <c r="L10" s="18">
+        <v>10</v>
+      </c>
+      <c r="M10" s="15">
         <v>828.94</v>
       </c>
-      <c r="N10" s="20">
-        <v>10</v>
-      </c>
-      <c r="O10" s="20">
+      <c r="N10" s="18">
+        <v>10</v>
+      </c>
+      <c r="O10" s="18">
         <v>828.93700000000001</v>
       </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="27">
+      <c r="P10" s="18"/>
+      <c r="Q10" s="25">
         <f t="shared" si="3"/>
         <v>-3.6190797886973073E-6</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="U10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="6">
-        <v>10</v>
-      </c>
-      <c r="W10" s="15">
+      <c r="V10" s="4">
+        <v>10</v>
+      </c>
+      <c r="W10" s="13">
         <v>1139.82</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10" s="4">
         <v>11</v>
       </c>
-      <c r="Y10" s="29">
+      <c r="Y10" s="27">
         <v>1135.73</v>
       </c>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="7">
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="5">
         <f t="shared" si="4"/>
         <v>-3.5882858696986526E-3</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>5</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>441.3</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="20">
         <v>4</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="18">
         <v>460.5</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="3">
+      <c r="F11" s="19"/>
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>4.3507817811012886E-2</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="6">
-        <v>10</v>
-      </c>
-      <c r="M11" s="15">
+      <c r="L11" s="4">
+        <v>10</v>
+      </c>
+      <c r="M11" s="13">
         <v>828.94</v>
       </c>
-      <c r="N11" s="6">
-        <v>10</v>
-      </c>
-      <c r="O11" s="6">
+      <c r="N11" s="4">
+        <v>10</v>
+      </c>
+      <c r="O11" s="4">
         <v>828.93700000000001</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="28">
+      <c r="P11" s="4"/>
+      <c r="Q11" s="26">
         <f t="shared" si="3"/>
         <v>-3.6190797886973073E-6</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>4</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <v>444.1</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="18">
         <v>4</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <v>445.8</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="3">
+      <c r="F12" s="19"/>
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>3.8279666741724578E-3</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>5</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <v>428.8</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>4</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="18">
         <v>429.7</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="3">
+      <c r="F13" s="19"/>
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>2.0988805970148725E-3</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <v>4</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="15">
         <v>393</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="18">
         <v>4</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="18">
         <v>394.1</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="3">
+      <c r="F14" s="19"/>
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>2.7989821882952234E-3</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="G15" s="4"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="14">
         <v>20</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="15">
         <v>1637.7</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="20">
         <v>19</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="18">
         <v>1677.6</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="5">
+      <c r="F17" s="18"/>
+      <c r="G17" s="3">
         <f>(E17-C17)/C17</f>
         <v>2.4363436526836334E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="14">
         <v>18</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="15">
         <v>1466.6</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="20">
         <v>17</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <v>1514.5</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="5">
+      <c r="F18" s="18"/>
+      <c r="G18" s="3">
         <f t="shared" ref="G18:G28" si="5">(E18-C18)/C18</f>
         <v>3.2660575480703731E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="14">
         <v>14</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="15">
         <v>1208.7</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="18">
         <v>14</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="18">
         <v>1255.2</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="5">
+      <c r="F19" s="18"/>
+      <c r="G19" s="3">
         <f t="shared" si="5"/>
         <v>3.8471084636386196E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="14">
         <v>11</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="18">
         <v>11</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="18">
         <v>1038.7</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="5">
+      <c r="F20" s="18"/>
+      <c r="G20" s="3">
         <v>6.9169999999999995E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="14">
         <v>15</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="15">
         <v>1355.3</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="20">
         <v>14</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="18">
         <v>1393.6</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="5">
+      <c r="F21" s="18"/>
+      <c r="G21" s="3">
         <f t="shared" si="5"/>
         <v>2.8259425957352584E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="14">
         <v>13</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="15">
         <v>1234.5999999999999</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="18">
         <v>13</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="18">
         <v>1283.7</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="5">
+      <c r="F22" s="18"/>
+      <c r="G22" s="3">
         <f t="shared" si="5"/>
         <v>3.9769965980884607E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="18">
         <v>11</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="15">
         <v>1064.5999999999999</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="18">
         <v>11</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="18">
         <v>1130.0999999999999</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="5">
+      <c r="F23" s="18"/>
+      <c r="G23" s="3">
         <f t="shared" si="5"/>
         <v>6.1525455570167205E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="20">
+      <c r="A24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="18">
         <v>9</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="15">
         <v>960.88</v>
       </c>
-      <c r="D24" s="20">
-        <v>10</v>
-      </c>
-      <c r="E24" s="20">
+      <c r="D24" s="18">
+        <v>10</v>
+      </c>
+      <c r="E24" s="18">
         <v>964.91499999999996</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="5">
+      <c r="F24" s="18"/>
+      <c r="G24" s="3">
         <f t="shared" si="5"/>
         <v>4.1992756639746571E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="18">
         <v>11</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="15">
         <v>1194.73</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="18">
         <v>12</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="18">
         <v>1194.47</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="5">
+      <c r="F25" s="18"/>
+      <c r="G25" s="3">
         <f t="shared" si="5"/>
         <v>-2.1762239167007685E-4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="20">
-        <v>10</v>
-      </c>
-      <c r="C26" s="17">
+      <c r="B26" s="18">
+        <v>10</v>
+      </c>
+      <c r="C26" s="15">
         <v>1118.5899999999999</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <v>12</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <v>1131.6199999999999</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="5">
+      <c r="F26" s="18"/>
+      <c r="G26" s="3">
         <f t="shared" si="5"/>
         <v>1.1648593318374001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="20">
-        <v>10</v>
-      </c>
-      <c r="C27" s="17">
+      <c r="B27" s="18">
+        <v>10</v>
+      </c>
+      <c r="C27" s="15">
         <v>1096.72</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="18">
         <v>11</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <v>1145.47</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="5">
+      <c r="F27" s="18"/>
+      <c r="G27" s="3">
         <f t="shared" si="5"/>
         <v>4.4450725800568969E-2</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>9</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <v>982.14</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>11</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <v>1004.68</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7">
+      <c r="F28" s="4"/>
+      <c r="G28" s="5">
         <f t="shared" si="5"/>
         <v>2.2949884945119802E-2</v>
       </c>

</xml_diff>